<commit_message>
Mockaroo api has been tested with SpartansApi
</commit_message>
<xml_diff>
--- a/src/test/resources/dummy_spartans.xlsx
+++ b/src/test/resources/dummy_spartans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optional_API_Tests\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3356DF-6BF0-4983-8F77-2DA984230A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B17FA41-7443-4F3C-9579-CE8C03AFC18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -41,30 +41,6 @@
   </si>
   <si>
     <t>Female</t>
-  </si>
-  <si>
-    <t>Derby</t>
-  </si>
-  <si>
-    <t>Birk</t>
-  </si>
-  <si>
-    <t>Elliot</t>
-  </si>
-  <si>
-    <t>Araldo</t>
-  </si>
-  <si>
-    <t>Anton</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>Ryley</t>
-  </si>
-  <si>
-    <t>Wash</t>
   </si>
 </sst>
 </file>
@@ -414,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -457,95 +433,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>6923378501</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>6679321548</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>6322389904</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>9844079148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>6335213996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>9521027878</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>6389681518</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>6786680607</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>9165979049</v>
+        <v>6923378500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>